<commit_message>
Actualización de cambios: integracion Mercado Pago y Tickets CRM de Zoho.
</commit_message>
<xml_diff>
--- a/uploads/ProductosDisponiblesAMW.xlsx
+++ b/uploads/ProductosDisponiblesAMW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP-IT\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EF521F-634C-4F00-85D9-0C14030634A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44024108-3C54-4E07-B12B-1D0FA0960318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="615" windowWidth="15375" windowHeight="10305" xr2:uid="{4C32EE9F-18FA-4DE2-8227-33A011D4D898}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4C32EE9F-18FA-4DE2-8227-33A011D4D898}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,45 +34,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+  <si>
+    <t> text</t>
+  </si>
+  <si>
+    <t>subText</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>stockDisponible</t>
+  </si>
+  <si>
+    <t>Single Vineyard</t>
+  </si>
+  <si>
+    <t>Cabernet (x6)</t>
+  </si>
+  <si>
+    <t>Almarada</t>
+  </si>
+  <si>
+    <t>Malbec (x6)</t>
+  </si>
+  <si>
+    <t>Chardonay (x6)</t>
+  </si>
+  <si>
+    <t>Núcleo3</t>
+  </si>
   <si>
     <t> image</t>
-  </si>
-  <si>
-    <t> text</t>
-  </si>
-  <si>
-    <t>subText</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>stockDisponible</t>
-  </si>
-  <si>
-    <t>malbec</t>
-  </si>
-  <si>
-    <t>/assets/p2-c159def9.png</t>
-  </si>
-  <si>
-    <t>vino2</t>
-  </si>
-  <si>
-    <t>vino3</t>
-  </si>
-  <si>
-    <t>cabernet</t>
-  </si>
-  <si>
-    <t>/assets/p2-c159de59.png</t>
-  </si>
-  <si>
-    <t>vino4</t>
-  </si>
-  <si>
-    <t>sauvignon blanc</t>
   </si>
 </sst>
 </file>
@@ -424,85 +418,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C502E8-6952-4092-862F-306D3A0A0A14}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D2">
-        <v>99</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>150</v>
+        <v>27000</v>
       </c>
       <c r="D3">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>599</v>
+        <v>50</v>
       </c>
       <c r="D4">
-        <v>150</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1000000</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>7000000</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>